<commit_message>
update dmn unit test
</commit_message>
<xml_diff>
--- a/dmn.tool/docs/DMN.xlsx
+++ b/dmn.tool/docs/DMN.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>input</t>
   </si>
@@ -184,6 +184,10 @@
   </si>
   <si>
     <t>dependency: T2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -239,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -269,6 +273,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -554,7 +561,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -664,7 +671,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -764,7 +771,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -834,30 +841,30 @@
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
+      <c r="E3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>40</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -868,11 +875,11 @@
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
       <c r="H6" s="5" t="s">
         <v>32</v>
       </c>

</xml_diff>